<commit_message>
Data list npy generated
</commit_message>
<xml_diff>
--- a/Character List.xlsx
+++ b/Character List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moe\Documents\GitHub\FP-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC29B0A9-2660-439C-84AA-23C9B08B5449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABB5E9-822B-4D8B-A77E-99438E27614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17175" yWindow="5310" windowWidth="14610" windowHeight="8325" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
+    <workbookView xWindow="-20520" yWindow="4620" windowWidth="19710" windowHeight="11760" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">	ඔ</t>
   </si>
   <si>
-    <t xml:space="preserve">	ඕ</t>
-  </si>
-  <si>
     <t>ක</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>ළ</t>
+  </si>
+  <si>
+    <t>ඕ</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F33FDE7-CE2C-4511-A4EC-85EC3BA39B35}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Data list npy generated"
This reverts commit 5a2c3911d35eb7154ee8797f54807f31b5700ac1.
</commit_message>
<xml_diff>
--- a/Character List.xlsx
+++ b/Character List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moe\Documents\GitHub\FP-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABB5E9-822B-4D8B-A77E-99438E27614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC29B0A9-2660-439C-84AA-23C9B08B5449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="4620" windowWidth="19710" windowHeight="11760" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
+    <workbookView xWindow="-17175" yWindow="5310" windowWidth="14610" windowHeight="8325" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,6 +68,9 @@
     <t xml:space="preserve">	ඔ</t>
   </si>
   <si>
+    <t xml:space="preserve">	ඕ</t>
+  </si>
+  <si>
     <t>ක</t>
   </si>
   <si>
@@ -126,9 +129,6 @@
   </si>
   <si>
     <t>ළ</t>
-  </si>
-  <si>
-    <t>ඕ</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F33FDE7-CE2C-4511-A4EC-85EC3BA39B35}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Data list npy generated""
This reverts commit 0638fa31237a13785d5fa5c1fbbcff214d4a25d6.
</commit_message>
<xml_diff>
--- a/Character List.xlsx
+++ b/Character List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moe\Documents\GitHub\FP-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC29B0A9-2660-439C-84AA-23C9B08B5449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABB5E9-822B-4D8B-A77E-99438E27614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17175" yWindow="5310" windowWidth="14610" windowHeight="8325" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
+    <workbookView xWindow="-20520" yWindow="4620" windowWidth="19710" windowHeight="11760" xr2:uid="{E2A6BD15-E70B-4B0A-8A51-5130533F33A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">	ඔ</t>
   </si>
   <si>
-    <t xml:space="preserve">	ඕ</t>
-  </si>
-  <si>
     <t>ක</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>ළ</t>
+  </si>
+  <si>
+    <t>ඕ</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F33FDE7-CE2C-4511-A4EC-85EC3BA39B35}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>